<commit_message>
Release MHD 4.2.2 close #419
</commit_message>
<xml_diff>
--- a/ITI/MHD/AssociationTypeVsRelatesTo.xlsx
+++ b/ITI/MHD/AssociationTypeVsRelatesTo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.2.1</t>
+    <t>4.2.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -72,7 +72,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>null (https://www.ihe.net/ihe_domains/it_infrastructure/)</t>
+  </si>
+  <si>
+    <t>null (iti@ihe.net)</t>
+  </si>
+  <si>
+    <t>IHE IT Infrastructure Technical Committee (iti@ihe.net)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -381,7 +387,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -389,36 +395,36 @@
         <v>18</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -437,113 +443,113 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s" s="1">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s" s="1">
         <v>30</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2"/>
     </row>

</xml_diff>